<commit_message>
Save as PDF and Email functionality
</commit_message>
<xml_diff>
--- a/data/Aggregated Monthly Infographic - Hyperlinks.xlsx
+++ b/data/Aggregated Monthly Infographic - Hyperlinks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpgplc-my.sharepoint.com/personal/hard_parikh_compass-usa_com/Documents/Desktop/infographic automation/Infographic-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{8266D76D-8560-4BF9-ACF6-270095CD97FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D58CF8D7-0F12-4BCD-B892-B0F45FFCBEAB}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_29D9C139D5E99B3EDBDB3111595ED87656CD94E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F579E7E-A9C7-4EAE-9431-5F829DAF3629}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,19 +53,16 @@
     <t>Order Accuracy</t>
   </si>
   <si>
-    <t>Ordering Experience</t>
+    <t>Customer Service</t>
   </si>
   <si>
-    <t>Customer Service</t>
+    <t>Food</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.######"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,13 +112,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,11 +450,11 @@
         <v>2024</v>
       </c>
       <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f>"178"</f>
-        <v>178</v>
+        <v>10</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"125"</f>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -470,11 +465,11 @@
         <v>2024</v>
       </c>
       <c r="C3">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f>"175"</f>
-        <v>175</v>
+        <v>10</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"121"</f>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -485,11 +480,11 @@
         <v>2024</v>
       </c>
       <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="str">
-        <f>"95.72"</f>
-        <v>95.72</v>
+        <v>10</v>
+      </c>
+      <c r="D4" t="str">
+        <f>"96.42"</f>
+        <v>96.42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -500,11 +495,11 @@
         <v>2024</v>
       </c>
       <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f>"14"</f>
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="D5" t="str">
+        <f>"7"</f>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -515,11 +510,11 @@
         <v>2024</v>
       </c>
       <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>"0.08"</f>
-        <v>0.08</v>
+        <v>10</v>
+      </c>
+      <c r="D6" t="str">
+        <f>"0.06"</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -530,11 +525,11 @@
         <v>2024</v>
       </c>
       <c r="C7">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f>"661"</f>
-        <v>661</v>
+        <v>10</v>
+      </c>
+      <c r="D7" t="str">
+        <f>"378"</f>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -545,11 +540,11 @@
         <v>2024</v>
       </c>
       <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f>"2.7"</f>
-        <v>2.7</v>
+        <v>10</v>
+      </c>
+      <c r="D8" t="str">
+        <f>"2.03"</f>
+        <v>2.03</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -560,11 +555,11 @@
         <v>2024</v>
       </c>
       <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f>"152"</f>
-        <v>152</v>
+        <v>10</v>
+      </c>
+      <c r="D9" t="str">
+        <f>"45"</f>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -575,11 +570,11 @@
         <v>2024</v>
       </c>
       <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f>"3.47"</f>
-        <v>3.47</v>
+        <v>10</v>
+      </c>
+      <c r="D10" t="str">
+        <f>"2.71"</f>
+        <v>2.71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -590,11 +585,11 @@
         <v>2024</v>
       </c>
       <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f>"7"</f>
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D11" t="str">
+        <f>"8"</f>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -605,9 +600,9 @@
         <v>2024</v>
       </c>
       <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D12" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
@@ -620,11 +615,11 @@
         <v>2024</v>
       </c>
       <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f>"32"</f>
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="D13" t="str">
+        <f>"16"</f>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -635,11 +630,11 @@
         <v>2024</v>
       </c>
       <c r="C14">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f>"49"</f>
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="D14" t="str">
+        <f>"40"</f>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -650,11 +645,11 @@
         <v>2024</v>
       </c>
       <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15" s="2" t="str">
-        <f>"15"</f>
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="D15" t="str">
+        <f>"14"</f>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -665,11 +660,11 @@
         <v>2024</v>
       </c>
       <c r="C16">
-        <v>9</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f>"42"</f>
-        <v>42</v>
+        <v>10</v>
+      </c>
+      <c r="D16" t="str">
+        <f>"21"</f>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -680,11 +675,11 @@
         <v>2024</v>
       </c>
       <c r="C17">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f>"11"</f>
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D17" t="str">
+        <f>"53"</f>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -695,11 +690,11 @@
         <v>2024</v>
       </c>
       <c r="C18">
-        <v>9</v>
-      </c>
-      <c r="D18" s="2" t="str">
-        <f>"4,002"</f>
-        <v>4,002</v>
+        <v>10</v>
+      </c>
+      <c r="D18" t="str">
+        <f>"4,621"</f>
+        <v>4,621</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -710,11 +705,11 @@
         <v>2024</v>
       </c>
       <c r="C19">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f>"1,894"</f>
-        <v>1,894</v>
+        <v>10</v>
+      </c>
+      <c r="D19" t="str">
+        <f>"1,883"</f>
+        <v>1,883</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -725,11 +720,11 @@
         <v>2024</v>
       </c>
       <c r="C20">
-        <v>9</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f>"431"</f>
-        <v>431</v>
+        <v>10</v>
+      </c>
+      <c r="D20" t="str">
+        <f>"493"</f>
+        <v>493</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -740,11 +735,11 @@
         <v>2024</v>
       </c>
       <c r="C21">
-        <v>9</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f>"987"</f>
-        <v>987</v>
+        <v>10</v>
+      </c>
+      <c r="D21" t="str">
+        <f>"1,011"</f>
+        <v>1,011</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -755,11 +750,11 @@
         <v>2024</v>
       </c>
       <c r="C22">
-        <v>9</v>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f>"475"</f>
-        <v>475</v>
+        <v>10</v>
+      </c>
+      <c r="D22" t="str">
+        <f>"379"</f>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -770,11 +765,11 @@
         <v>2024</v>
       </c>
       <c r="C23">
-        <v>9</v>
-      </c>
-      <c r="D23" s="3" t="str">
-        <f>"0.227561"</f>
-        <v>0.227561</v>
+        <v>10</v>
+      </c>
+      <c r="D23" t="str">
+        <f>"0.261816"</f>
+        <v>0.261816</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -785,11 +780,11 @@
         <v>2024</v>
       </c>
       <c r="C24">
-        <v>9</v>
-      </c>
-      <c r="D24" s="3" t="str">
-        <f>"0.521119"</f>
-        <v>0.521119</v>
+        <v>10</v>
+      </c>
+      <c r="D24" t="str">
+        <f>"0.536909"</f>
+        <v>0.536909</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -800,11 +795,11 @@
         <v>2024</v>
       </c>
       <c r="C25">
-        <v>9</v>
-      </c>
-      <c r="D25" s="3" t="str">
-        <f>"0.250792"</f>
-        <v>0.250792</v>
+        <v>10</v>
+      </c>
+      <c r="D25" t="str">
+        <f>"0.201275"</f>
+        <v>0.201275</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -815,11 +810,11 @@
         <v>2024</v>
       </c>
       <c r="C26">
-        <v>9</v>
-      </c>
-      <c r="D26" s="2" t="str">
-        <f>"249"</f>
-        <v>249</v>
+        <v>10</v>
+      </c>
+      <c r="D26" t="str">
+        <f>"432"</f>
+        <v>432</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
@@ -833,11 +828,11 @@
         <v>2024</v>
       </c>
       <c r="C27">
-        <v>9</v>
-      </c>
-      <c r="D27" s="2" t="str">
-        <f>"235"</f>
-        <v>235</v>
+        <v>10</v>
+      </c>
+      <c r="D27" t="str">
+        <f>"394"</f>
+        <v>394</v>
       </c>
       <c r="E27" t="s">
         <v>6</v>
@@ -851,11 +846,11 @@
         <v>2024</v>
       </c>
       <c r="C28">
-        <v>9</v>
-      </c>
-      <c r="D28" s="2" t="str">
-        <f>"217"</f>
-        <v>217</v>
+        <v>10</v>
+      </c>
+      <c r="D28" t="str">
+        <f>"379"</f>
+        <v>379</v>
       </c>
       <c r="E28" t="s">
         <v>7</v>
@@ -869,11 +864,11 @@
         <v>2024</v>
       </c>
       <c r="C29">
-        <v>9</v>
-      </c>
-      <c r="D29" s="2" t="str">
-        <f>"645"</f>
-        <v>645</v>
+        <v>10</v>
+      </c>
+      <c r="D29" t="str">
+        <f>"648"</f>
+        <v>648</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -884,9 +879,9 @@
         <v>2024</v>
       </c>
       <c r="C30">
-        <v>9</v>
-      </c>
-      <c r="D30" s="3" t="str">
+        <v>10</v>
+      </c>
+      <c r="D30" t="str">
         <f>"0.85"</f>
         <v>0.85</v>
       </c>
@@ -899,9 +894,9 @@
         <v>2024</v>
       </c>
       <c r="C31">
-        <v>9</v>
-      </c>
-      <c r="D31" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D31" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -914,9 +909,9 @@
         <v>2024</v>
       </c>
       <c r="C32">
-        <v>9</v>
-      </c>
-      <c r="D32" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D32" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -929,9 +924,9 @@
         <v>2024</v>
       </c>
       <c r="C33">
-        <v>9</v>
-      </c>
-      <c r="D33" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D33" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -944,9 +939,9 @@
         <v>2024</v>
       </c>
       <c r="C34">
-        <v>9</v>
-      </c>
-      <c r="D34" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D34" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -959,9 +954,9 @@
         <v>2024</v>
       </c>
       <c r="C35">
-        <v>9</v>
-      </c>
-      <c r="D35" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D35" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -974,9 +969,9 @@
         <v>2024</v>
       </c>
       <c r="C36">
-        <v>9</v>
-      </c>
-      <c r="D36" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D36" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -989,9 +984,9 @@
         <v>2024</v>
       </c>
       <c r="C37">
-        <v>9</v>
-      </c>
-      <c r="D37" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D37" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1004,9 +999,9 @@
         <v>2024</v>
       </c>
       <c r="C38">
-        <v>9</v>
-      </c>
-      <c r="D38" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D38" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1019,9 +1014,9 @@
         <v>2024</v>
       </c>
       <c r="C39">
-        <v>9</v>
-      </c>
-      <c r="D39" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D39" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1034,9 +1029,9 @@
         <v>2024</v>
       </c>
       <c r="C40">
-        <v>9</v>
-      </c>
-      <c r="D40" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D40" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1049,9 +1044,9 @@
         <v>2024</v>
       </c>
       <c r="C41">
-        <v>9</v>
-      </c>
-      <c r="D41" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D41" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1064,9 +1059,9 @@
         <v>2024</v>
       </c>
       <c r="C42">
-        <v>9</v>
-      </c>
-      <c r="D42" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D42" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1079,9 +1074,9 @@
         <v>2024</v>
       </c>
       <c r="C43">
-        <v>9</v>
-      </c>
-      <c r="D43" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D43" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1094,9 +1089,9 @@
         <v>2024</v>
       </c>
       <c r="C44">
-        <v>9</v>
-      </c>
-      <c r="D44" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D44" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1109,9 +1104,9 @@
         <v>2024</v>
       </c>
       <c r="C45">
-        <v>9</v>
-      </c>
-      <c r="D45" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D45" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1124,9 +1119,9 @@
         <v>2024</v>
       </c>
       <c r="C46">
-        <v>9</v>
-      </c>
-      <c r="D46" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D46" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1139,9 +1134,9 @@
         <v>2024</v>
       </c>
       <c r="C47">
-        <v>9</v>
-      </c>
-      <c r="D47" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D47" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1154,9 +1149,9 @@
         <v>2024</v>
       </c>
       <c r="C48">
-        <v>9</v>
-      </c>
-      <c r="D48" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D48" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1169,9 +1164,9 @@
         <v>2024</v>
       </c>
       <c r="C49">
-        <v>9</v>
-      </c>
-      <c r="D49" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D49" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1184,9 +1179,9 @@
         <v>2024</v>
       </c>
       <c r="C50">
-        <v>9</v>
-      </c>
-      <c r="D50" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D50" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1199,9 +1194,9 @@
         <v>2024</v>
       </c>
       <c r="C51">
-        <v>9</v>
-      </c>
-      <c r="D51" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D51" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1214,9 +1209,9 @@
         <v>2024</v>
       </c>
       <c r="C52">
-        <v>9</v>
-      </c>
-      <c r="D52" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D52" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1229,9 +1224,9 @@
         <v>2024</v>
       </c>
       <c r="C53">
-        <v>9</v>
-      </c>
-      <c r="D53" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D53" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1244,9 +1239,9 @@
         <v>2024</v>
       </c>
       <c r="C54">
-        <v>9</v>
-      </c>
-      <c r="D54" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D54" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>
@@ -1259,9 +1254,9 @@
         <v>2024</v>
       </c>
       <c r="C55">
-        <v>9</v>
-      </c>
-      <c r="D55" s="2" t="str">
+        <v>10</v>
+      </c>
+      <c r="D55" t="str">
         <f>"0"</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Final changes for the phase/version 1
</commit_message>
<xml_diff>
--- a/data/Aggregated Monthly Infographic - Hyperlinks.xlsx
+++ b/data/Aggregated Monthly Infographic - Hyperlinks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpgplc-my.sharepoint.com/personal/hard_parikh_compass-usa_com/Documents/Desktop/infographic automation/Infographic-Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="11_29D9C139D5E99B3EDBDB3111595ED87656CD94E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F579E7E-A9C7-4EAE-9431-5F829DAF3629}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_3A49412ED5F9124FD7BA2C11595ED87656CDB4EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C72036C-6E12-4D62-85E9-E6A81341C1D0}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregated Monthly Infographic" sheetId="1" r:id="rId1"/>
@@ -453,8 +453,8 @@
         <v>10</v>
       </c>
       <c r="D2" t="str">
-        <f>"125"</f>
-        <v>125</v>
+        <f>"131"</f>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -468,8 +468,8 @@
         <v>10</v>
       </c>
       <c r="D3" t="str">
-        <f>"121"</f>
-        <v>121</v>
+        <f>"127"</f>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -483,8 +483,8 @@
         <v>10</v>
       </c>
       <c r="D4" t="str">
-        <f>"96.42"</f>
-        <v>96.42</v>
+        <f>"96.47"</f>
+        <v>96.47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -513,8 +513,8 @@
         <v>10</v>
       </c>
       <c r="D6" t="str">
-        <f>"0.06"</f>
-        <v>0.06</v>
+        <f>"0.05"</f>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -528,8 +528,8 @@
         <v>10</v>
       </c>
       <c r="D7" t="str">
-        <f>"378"</f>
-        <v>378</v>
+        <f>"389"</f>
+        <v>389</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -543,8 +543,8 @@
         <v>10</v>
       </c>
       <c r="D8" t="str">
-        <f>"2.03"</f>
-        <v>2.03</v>
+        <f>"2.17"</f>
+        <v>2.17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -558,8 +558,8 @@
         <v>10</v>
       </c>
       <c r="D9" t="str">
-        <f>"45"</f>
-        <v>45</v>
+        <f>"56"</f>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -573,8 +573,8 @@
         <v>10</v>
       </c>
       <c r="D10" t="str">
-        <f>"2.71"</f>
-        <v>2.71</v>
+        <f>"3.6"</f>
+        <v>3.6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -663,8 +663,8 @@
         <v>10</v>
       </c>
       <c r="D16" t="str">
-        <f>"21"</f>
-        <v>21</v>
+        <f>"22"</f>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -678,8 +678,8 @@
         <v>10</v>
       </c>
       <c r="D17" t="str">
-        <f>"53"</f>
-        <v>53</v>
+        <f>"42"</f>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>